<commit_message>
Criterion E is generated with updated knowledge base
</commit_message>
<xml_diff>
--- a/ClientInput/CSSE-allprograms-outcome-mappings-20240913.xlsx
+++ b/ClientInput/CSSE-allprograms-outcome-mappings-20240913.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23076078_student_uwa_edu_au/Documents/2024 Semester 2/CITS5206/Staging/Client Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shalu/Desktop/accreditation_mapper_group_12_capstone_project/ClientInput/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{8E1B51B8-FD03-F149-B31B-7454C4CAEEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE6ECB82-1079-4224-B6B5-851A980A19EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC5ECD0-158A-074D-970F-3CF7C4A39A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B05868E8-B553-48B4-AD0E-A3C024BB8F88}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16860" activeTab="2" xr2:uid="{B05868E8-B553-48B4-AD0E-A3C024BB8F88}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
     <sheet name="Outcomes Mappings" sheetId="1" r:id="rId2"/>
-    <sheet name="Programs Details" sheetId="2" r:id="rId3"/>
+    <sheet name="Unit Details" sheetId="2" r:id="rId3"/>
     <sheet name="Unit Outcomes" sheetId="5" r:id="rId4"/>
     <sheet name="Outcomes Details" sheetId="3" r:id="rId5"/>
     <sheet name="SFIA justifications" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Programs Details'!$A$1:$N$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Unit Details'!$A$1:$N$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Unit Outcomes'!$A$1:$D$64</definedName>
-    <definedName name="_xlcn.WorksheetConnection_OutcomesMappingsA2H311" hidden="1">'Outcomes Mappings'!$A$1:$F$30</definedName>
+    <definedName name="_xlcn.WorksheetConnection_OutcomesMappingsA2H31" hidden="1">'Outcomes Mappings'!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -67,7 +67,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_OutcomesMappingsA2H311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_OutcomesMappingsA2H31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1803,7 +1803,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2621,27 +2621,27 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="137.1328125" customWidth="1"/>
+    <col min="2" max="2" width="137.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="25"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2649,29 +2649,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25"/>
       <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2679,53 +2679,53 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2733,141 +2733,141 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="25"/>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25"/>
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="25"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="25"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="25"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="25"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="25"/>
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="25"/>
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="25"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="25"/>
       <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="25"/>
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="25"/>
       <c r="B31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="25"/>
       <c r="B34" s="25"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="25"/>
       <c r="B35" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18.95" customHeight="1">
+    <row r="36" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25"/>
       <c r="B36" s="55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="18.95" customHeight="1">
+    <row r="37" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25"/>
       <c r="B37" s="55" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="25"/>
       <c r="B38" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="25"/>
       <c r="B39" s="25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="25"/>
       <c r="B40" s="25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="25"/>
       <c r="B41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="25"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>37</v>
       </c>
@@ -2875,142 +2875,142 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="15.95" customHeight="1">
+    <row r="50" spans="2:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>66</v>
       </c>
@@ -3018,92 +3018,92 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>85</v>
       </c>
@@ -3111,115 +3111,115 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="2:2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="2:2">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="2:2">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="2:2">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="102" spans="2:2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="2:2">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="2:2">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="2:2">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="2:2">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="2:2">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="2:2">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="2:2">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="2:2">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="2:2">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B115" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" s="4"/>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>108</v>
       </c>
@@ -3227,12 +3227,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" s="4" t="s">
         <v>111</v>
       </c>
@@ -3246,23 +3246,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98474689-BC2D-45B6-93FB-400891FC5F0E}">
   <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="38.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" customWidth="1"/>
     <col min="5" max="5" width="10" style="44" customWidth="1"/>
-    <col min="6" max="6" width="90.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="73.3984375" customWidth="1"/>
-    <col min="8" max="8" width="44.86328125" customWidth="1"/>
+    <col min="6" max="6" width="90.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="73.33203125" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>112</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>119</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42.75">
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>119</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57" customHeight="1">
+    <row r="4" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>119</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.5">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>119</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="42.75">
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>119</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.75">
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>119</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42.75">
+    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>119</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>119</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="57">
+    <row r="10" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>119</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>119</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.5">
+    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>119</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.5">
+    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>119</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="63" customHeight="1">
+    <row r="14" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>119</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>168</v>
       </c>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="G15" s="32"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>168</v>
       </c>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="G16" s="32"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>168</v>
       </c>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="G17" s="32"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>168</v>
       </c>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="G18" s="32"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>168</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="G19" s="32"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>168</v>
       </c>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="G20" s="32"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>168</v>
       </c>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G21" s="32"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>168</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="G22" s="32"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>168</v>
       </c>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="G23" s="32"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>168</v>
       </c>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="G24" s="32"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>168</v>
       </c>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="G25" s="32"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
         <v>168</v>
       </c>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="G26" s="32"/>
     </row>
-    <row r="27" spans="1:7" ht="28.5">
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>168</v>
       </c>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
         <v>168</v>
       </c>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="1:7" ht="28.5">
+    <row r="29" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
         <v>168</v>
       </c>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="G29" s="32"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
         <v>168</v>
       </c>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="G30" s="32"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
         <v>168</v>
       </c>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="G31" s="32"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
         <v>168</v>
       </c>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="G32" s="32"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
         <v>168</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="G33" s="32"/>
     </row>
-    <row r="34" spans="1:7" ht="14.65" thickBot="1">
+    <row r="34" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
         <v>168</v>
       </c>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="G34" s="32"/>
     </row>
-    <row r="35" spans="1:7" ht="14.65" thickBot="1">
+    <row r="35" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>168</v>
       </c>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="G35" s="32"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>168</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="G36" s="32"/>
     </row>
-    <row r="37" spans="1:7" ht="18.95" customHeight="1">
+    <row r="37" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>168</v>
       </c>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="G37" s="32"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>168</v>
       </c>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="G38" s="32"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>168</v>
       </c>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="G39" s="32"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="31" t="s">
         <v>168</v>
       </c>
@@ -4104,7 +4104,7 @@
       </c>
       <c r="G40" s="32"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>168</v>
       </c>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="G41" s="32"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>168</v>
       </c>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="G42" s="32"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>168</v>
       </c>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="G43" s="32"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>168</v>
       </c>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="G44" s="32"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>168</v>
       </c>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="G45" s="32"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="31" t="s">
         <v>168</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="F46" s="31"/>
       <c r="G46" s="32"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="31" t="s">
         <v>168</v>
       </c>
@@ -4243,7 +4243,7 @@
       <c r="F47" s="31"/>
       <c r="G47" s="32"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
         <v>168</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="F48" s="31"/>
       <c r="G48" s="32"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="31" t="s">
         <v>168</v>
       </c>
@@ -4277,7 +4277,7 @@
       <c r="F49" s="31"/>
       <c r="G49" s="32"/>
     </row>
-    <row r="50" spans="1:7" ht="27.75">
+    <row r="50" spans="1:7" ht="31" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>213</v>
       </c>
@@ -4296,7 +4296,7 @@
       </c>
       <c r="G50" s="32"/>
     </row>
-    <row r="51" spans="1:7" ht="27.75">
+    <row r="51" spans="1:7" ht="31" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>213</v>
       </c>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="G51" s="32"/>
     </row>
-    <row r="52" spans="1:7" ht="27.75">
+    <row r="52" spans="1:7" ht="31" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>213</v>
       </c>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="1:7" ht="176.25">
+    <row r="53" spans="1:7" ht="196" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>219</v>
       </c>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="G53" s="53"/>
     </row>
-    <row r="54" spans="1:7" ht="189.75">
+    <row r="54" spans="1:7" ht="211" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>219</v>
       </c>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>222</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>222</v>
       </c>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
         <v>222</v>
       </c>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="G57" s="53"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
         <v>222</v>
       </c>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
         <v>222</v>
       </c>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="G59" s="53"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
         <v>222</v>
       </c>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="G60" s="53"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
         <v>222</v>
       </c>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="G61" s="53"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="32" t="s">
         <v>222</v>
       </c>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="G62" s="53"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="32" t="s">
         <v>222</v>
       </c>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="G63" s="53"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
         <v>222</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="G64" s="53"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
         <v>222</v>
       </c>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="G65" s="32"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
         <v>222</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="G66" s="32"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
         <v>222</v>
       </c>
@@ -4619,7 +4619,7 @@
       </c>
       <c r="G67" s="32"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="32" t="s">
         <v>222</v>
       </c>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="G68" s="32"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
         <v>222</v>
       </c>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="G69" s="32"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="32" t="s">
         <v>222</v>
       </c>
@@ -4676,7 +4676,7 @@
       </c>
       <c r="G70" s="32"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="32" t="s">
         <v>222</v>
       </c>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="G71" s="32"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="32" t="s">
         <v>222</v>
       </c>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="G72" s="32"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="32" t="s">
         <v>222</v>
       </c>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="G73" s="32"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="32" t="s">
         <v>222</v>
       </c>
@@ -4752,7 +4752,7 @@
       </c>
       <c r="G74" s="32"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="32" t="s">
         <v>222</v>
       </c>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="G75" s="32"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="32" t="s">
         <v>222</v>
       </c>
@@ -4790,7 +4790,7 @@
       </c>
       <c r="G76" s="32"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="32" t="s">
         <v>222</v>
       </c>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="G77" s="32"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="32" t="s">
         <v>222</v>
       </c>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="G78" s="32"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="32" t="s">
         <v>222</v>
       </c>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="G79" s="32"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="32" t="s">
         <v>222</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="G80" s="32"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="32" t="s">
         <v>222</v>
       </c>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="G81" s="32"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="32" t="s">
         <v>222</v>
       </c>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="G82" s="32"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="32" t="s">
         <v>222</v>
       </c>
@@ -4923,7 +4923,7 @@
       </c>
       <c r="G83" s="32"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="32" t="s">
         <v>222</v>
       </c>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="G84" s="32"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="47" t="s">
         <v>168</v>
       </c>
@@ -4958,7 +4958,7 @@
       <c r="E85" s="42"/>
       <c r="F85" s="31"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="47" t="s">
         <v>168</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="E86" s="42"/>
       <c r="F86" s="31"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="47" t="s">
         <v>168</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="E87" s="42"/>
       <c r="F87" s="31"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="47" t="s">
         <v>168</v>
       </c>
@@ -5006,7 +5006,7 @@
       <c r="E88" s="42"/>
       <c r="F88" s="31"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="47" t="s">
         <v>168</v>
       </c>
@@ -5022,7 +5022,7 @@
       <c r="E89" s="42"/>
       <c r="F89" s="31"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="47" t="s">
         <v>168</v>
       </c>
@@ -5038,7 +5038,7 @@
       <c r="E90" s="42"/>
       <c r="F90" s="31"/>
     </row>
-    <row r="91" spans="1:7" s="2" customFormat="1">
+    <row r="91" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="29" t="s">
         <v>112</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="28.5">
+    <row r="92" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>241</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="28.5">
+    <row r="93" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="32" t="s">
         <v>244</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="32" t="s">
         <v>244</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
         <v>241</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
         <v>241</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>241</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="32" t="s">
         <v>241</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="32" t="s">
         <v>241</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="71.25">
+    <row r="100" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A100" s="32" t="s">
         <v>241</v>
       </c>
@@ -5243,7 +5243,7 @@
       <c r="G100" s="23"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" ht="28.5">
+    <row r="101" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="32" t="s">
         <v>241</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="42.75">
+    <row r="102" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="32" t="s">
         <v>241</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="45.95" customHeight="1">
+    <row r="103" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="32" t="s">
         <v>241</v>
       </c>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:8" ht="45.95" customHeight="1">
+    <row r="104" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="32" t="s">
         <v>241</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="45.95" customHeight="1">
+    <row r="105" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="32" t="s">
         <v>241</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="45.95" customHeight="1">
+    <row r="106" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="32" t="s">
         <v>241</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="45.95" customHeight="1">
+    <row r="107" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="32" t="s">
         <v>241</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="45.95" customHeight="1">
+    <row r="108" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="32" t="s">
         <v>241</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="195.95" customHeight="1">
+    <row r="109" spans="1:8" ht="196" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="32" t="s">
         <v>241</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="90.95" customHeight="1">
+    <row r="110" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="32" t="s">
         <v>241</v>
       </c>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:8" ht="45.95" customHeight="1">
+    <row r="111" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="32" t="s">
         <v>244</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="28.5">
+    <row r="112" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="32" t="s">
         <v>241</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="32" t="s">
         <v>241</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="32" t="s">
         <v>244</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="32" t="s">
         <v>244</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="28.5">
+    <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="32" t="s">
         <v>244</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="32" t="s">
         <v>244</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="118" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="32" t="s">
         <v>241</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" customHeight="1">
+    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="32" t="s">
         <v>241</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="32" t="s">
         <v>241</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="32" t="s">
         <v>241</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="85.5">
+    <row r="122" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A122" s="32" t="s">
         <v>244</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="156.75">
+    <row r="123" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A123" s="32" t="s">
         <v>241</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="28.5">
+    <row r="124" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="32" t="s">
         <v>241</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="57">
+    <row r="125" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A125" s="32" t="s">
         <v>244</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="57">
+    <row r="126" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A126" s="32" t="s">
         <v>244</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="57">
+    <row r="127" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A127" s="32" t="s">
         <v>241</v>
       </c>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7" ht="39" customHeight="1">
+    <row r="128" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="32" t="s">
         <v>244</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="28.5">
+    <row r="129" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="32" t="s">
         <v>241</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="28.5">
+    <row r="130" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="32" t="s">
         <v>241</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="32" t="s">
         <v>244</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="28.5">
+    <row r="132" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="32" t="s">
         <v>244</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="28.5">
+    <row r="133" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="32" t="s">
         <v>244</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="28.5">
+    <row r="134" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="32" t="s">
         <v>244</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="32" t="s">
         <v>241</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="32" t="s">
         <v>241</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="32" t="s">
         <v>241</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="66" customHeight="1">
+    <row r="138" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="32" t="s">
         <v>244</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="85.5">
+    <row r="139" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A139" s="32" t="s">
         <v>244</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="85.5">
+    <row r="140" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A140" s="32" t="s">
         <v>244</v>
       </c>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="1:7" ht="99.75">
+    <row r="141" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A141" s="32" t="s">
         <v>244</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="42.75">
+    <row r="142" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A142" s="32" t="s">
         <v>244</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="32"/>
       <c r="B143" s="32"/>
       <c r="C143" s="32"/>
@@ -6110,7 +6110,7 @@
       <c r="E143" s="42"/>
       <c r="F143" s="31"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="32" t="s">
         <v>307</v>
       </c>
@@ -6124,34 +6124,34 @@
         <v>309</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" s="1"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" s="1"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="1"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="1"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="1"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="1"/>
     </row>
   </sheetData>
@@ -6169,25 +6169,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4998F0D-B8E9-4116-BFF4-489EA6F19212}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="A24:B24"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
-    <col min="2" max="2" width="34.86328125" customWidth="1"/>
-    <col min="3" max="3" width="5.265625" customWidth="1"/>
-    <col min="4" max="4" width="4.73046875" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
-    <col min="6" max="9" width="15.86328125" customWidth="1"/>
-    <col min="10" max="11" width="22.265625" customWidth="1"/>
-    <col min="12" max="12" width="21.73046875" customWidth="1"/>
-    <col min="13" max="14" width="22.265625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="11" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="13" max="14" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="57">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>114</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>266</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>232</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>326</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>332</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>201</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>336</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>234</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>339</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>190</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>345</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>192</v>
       </c>
@@ -7040,7 +7040,7 @@
       </c>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>350</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>352</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>356</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>363</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>299</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>365</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>367</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>303</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>370</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>181</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>372</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>374</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>377</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>382</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>384</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>386</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>235</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>388</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>239</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>237</v>
       </c>
@@ -7786,14 +7786,14 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.3984375" customWidth="1"/>
-    <col min="3" max="3" width="90.73046875" customWidth="1"/>
-    <col min="4" max="4" width="27.265625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="90.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="71.25">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="71.25">
+    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="85.5">
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="180" customHeight="1">
+    <row r="5" spans="1:4" ht="180" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="114">
+    <row r="6" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="114">
+    <row r="7" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="156.75">
+    <row r="8" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="99.75">
+    <row r="9" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>266</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="156.75">
+    <row r="10" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>232</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="114">
+    <row r="11" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="156.75">
+    <row r="12" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>326</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>332</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>201</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>336</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="85.5">
+    <row r="19" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>234</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="99.75">
+    <row r="22" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>339</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -8039,7 +8039,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>190</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="156.75">
+    <row r="26" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>345</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>192</v>
       </c>
@@ -8082,7 +8082,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>350</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>352</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>356</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="128.25">
+    <row r="35" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="114">
+    <row r="39" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>363</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="228">
+    <row r="46" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>299</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>365</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>367</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="228">
+    <row r="49" spans="1:3" ht="256" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>303</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>370</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>181</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>372</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>374</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>377</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>382</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>384</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>386</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>235</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>388</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>239</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>237</v>
       </c>
@@ -8391,16 +8391,16 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.3984375" customWidth="1"/>
-    <col min="3" max="3" width="22.1328125" customWidth="1"/>
-    <col min="4" max="4" width="87.265625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="31.3984375" customWidth="1"/>
-    <col min="6" max="6" width="63.265625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="87.33203125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>112</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -8436,7 +8436,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>168</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="28.9">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="28.9">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>168</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="28.5">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>168</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="44.1" customHeight="1">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
@@ -8596,7 +8596,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="28.5">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>168</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" ht="28.5">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>168</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="27.75">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>168</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" ht="27.75">
+    <row r="16" spans="1:6" s="14" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>168</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="122.25">
+    <row r="17" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>450</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="54.75">
+    <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>450</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="81.75">
+    <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>450</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57">
+    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>450</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="54.75">
+    <row r="21" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>450</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="D22" s="6"/>
       <c r="E22" s="4"/>
@@ -8753,7 +8753,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="135.75">
+    <row r="23" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>450</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="108.75">
+    <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>450</v>
       </c>
@@ -8789,7 +8789,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="68.25">
+    <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>450</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="128.25">
+    <row r="26" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>450</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="171">
+    <row r="27" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>450</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="81.75">
+    <row r="28" spans="1:6" ht="91" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>450</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="114">
+    <row r="29" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>450</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="108.75">
+    <row r="30" spans="1:6" ht="121" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>450</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="57">
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>450</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.5">
+    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -8924,7 +8924,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="42.75">
+    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>213</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.5">
+    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>219</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="68.25">
+    <row r="36" spans="1:6" ht="76" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>222</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="81.75">
+    <row r="37" spans="1:6" ht="91" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>222</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="68.25">
+    <row r="38" spans="1:6" ht="61" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>222</v>
       </c>
@@ -9012,13 +9012,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.73046875" customWidth="1"/>
-    <col min="2" max="5" width="114.73046875" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="5" width="114.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>480</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="69.95" customHeight="1">
+    <row r="2" spans="1:2" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="93" customHeight="1">
+    <row r="3" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="57">
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="42.75">
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>198</v>
       </c>

</xml_diff>